<commit_message>
sql alchemy search updated
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -51,12 +49,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,58 +472,6 @@
         <v>7588476553</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>15</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>pranjalOrientation</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>8695847465</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>45016.41915509259</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>14</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>pranjalReception</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>7647563743</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>45016.41915509259</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>